<commit_message>
created Claudminity as a simple proj. use v2 RN
</commit_message>
<xml_diff>
--- a/cognitive_test_results.xlsx
+++ b/cognitive_test_results.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madma\Documents\zDrugMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{693093E8-9E74-429D-84A9-E7E38765DEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3856623E-4231-4088-A78C-018BE4A3CDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{0EBB6897-470D-46A5-95F9-4F5FAD9B2DC1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0EBB6897-470D-46A5-95F9-4F5FAD9B2DC1}"/>
   </bookViews>
   <sheets>
     <sheet name="cognitive_test_results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Date and Time</t>
   </si>
@@ -41,6 +54,12 @@
   </si>
   <si>
     <t>Total Subtraction Time (s)</t>
+  </si>
+  <si>
+    <t>sober</t>
+  </si>
+  <si>
+    <t>THC</t>
   </si>
 </sst>
 </file>
@@ -906,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F461D8B-DBFF-4F94-A845-BF692CC26C79}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A3" sqref="A3:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,59 +942,59 @@
     <col min="7" max="7" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <f>AVERAGE(B4:B8)</f>
-        <v>12.806666666666667</v>
+        <v>10.712</v>
       </c>
       <c r="C1" s="2">
         <f t="shared" ref="C1:G1" si="0">AVERAGE(C4:C8)</f>
-        <v>47.743333333333332</v>
+        <v>43.786000000000001</v>
       </c>
       <c r="D1" s="2">
         <f t="shared" si="0"/>
-        <v>12.143333333333333</v>
+        <v>9.548</v>
       </c>
       <c r="E1" s="2">
         <f t="shared" si="0"/>
-        <v>23.256666666666664</v>
+        <v>25.265999999999998</v>
       </c>
       <c r="F1" s="2">
         <f t="shared" si="0"/>
-        <v>8.3566666666666674</v>
+        <v>8.0139999999999993</v>
       </c>
       <c r="G1" s="2">
         <f t="shared" si="0"/>
-        <v>41.793333333333329</v>
+        <v>40.077999999999996</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
         <f>STDEV(B4:B8)/SQRT(COUNT(B4:B8))</f>
-        <v>4.12902059950191</v>
+        <v>2.6015080242044224</v>
       </c>
       <c r="C2" s="2">
         <f t="shared" ref="C2:G2" si="1">STDEV(C4:C8)/SQRT(COUNT(C4:C8))</f>
-        <v>4.6764742179457466</v>
+        <v>3.5538016264276817</v>
       </c>
       <c r="D2" s="2">
         <f t="shared" si="1"/>
-        <v>7.2504720152859328</v>
+        <v>4.2832714133008203</v>
       </c>
       <c r="E2" s="2">
         <f t="shared" si="1"/>
-        <v>1.500825698666497</v>
+        <v>1.8498070169614984</v>
       </c>
       <c r="F2" s="2">
         <f t="shared" si="1"/>
-        <v>1.0780280350920615</v>
+        <v>0.7309486986102377</v>
       </c>
       <c r="G2" s="2">
         <f t="shared" si="1"/>
-        <v>5.3807568653902687</v>
+        <v>3.6485029806757883</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -998,83 +1017,255 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>45464.98159722222</v>
+        <v>45464.983761574076</v>
+      </c>
+      <c r="B4">
+        <v>21.03</v>
+      </c>
+      <c r="C4">
+        <v>56.29</v>
+      </c>
+      <c r="D4">
+        <v>5.2</v>
+      </c>
+      <c r="E4">
+        <v>26</v>
+      </c>
+      <c r="F4">
+        <v>10.38</v>
+      </c>
+      <c r="G4">
+        <v>51.89</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>45464.983761574076</v>
+        <v>45465.918240740742</v>
       </c>
       <c r="B5">
-        <v>21.03</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="C5">
-        <v>56.29</v>
+        <v>40.18</v>
       </c>
       <c r="D5">
-        <v>5.2</v>
+        <v>4.59</v>
       </c>
       <c r="E5">
-        <v>26</v>
+        <v>22.94</v>
       </c>
       <c r="F5">
-        <v>10.38</v>
+        <v>7.99</v>
       </c>
       <c r="G5">
-        <v>51.89</v>
+        <v>39.97</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>45464.985474537039</v>
+        <v>45472.964467592596</v>
+      </c>
+      <c r="B6">
+        <v>9.35</v>
+      </c>
+      <c r="C6">
+        <v>46.76</v>
+      </c>
+      <c r="D6">
+        <v>26.64</v>
+      </c>
+      <c r="E6">
+        <v>20.83</v>
+      </c>
+      <c r="F6">
+        <v>6.7</v>
+      </c>
+      <c r="G6">
+        <v>33.520000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>45465.918240740742</v>
+        <v>45475.812881944446</v>
       </c>
       <c r="B7">
-        <v>8.0399999999999991</v>
+        <v>7.29</v>
       </c>
       <c r="C7">
-        <v>40.18</v>
+        <v>36.450000000000003</v>
       </c>
       <c r="D7">
-        <v>4.59</v>
+        <v>6.36</v>
       </c>
       <c r="E7">
-        <v>22.94</v>
+        <v>31.79</v>
       </c>
       <c r="F7">
-        <v>7.99</v>
+        <v>8.69</v>
       </c>
       <c r="G7">
-        <v>39.97</v>
+        <v>43.44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>45472.964467592596</v>
+        <v>45475.978101851855</v>
       </c>
       <c r="B8">
-        <v>9.35</v>
+        <v>7.85</v>
       </c>
       <c r="C8">
-        <v>46.76</v>
+        <v>39.25</v>
       </c>
       <c r="D8">
-        <v>26.64</v>
+        <v>4.95</v>
       </c>
       <c r="E8">
-        <v>20.83</v>
+        <v>24.77</v>
       </c>
       <c r="F8">
-        <v>6.7</v>
+        <v>6.31</v>
       </c>
       <c r="G8">
-        <v>33.520000000000003</v>
+        <v>31.57</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>45475.984467592592</v>
+      </c>
+      <c r="B9">
+        <v>8.57</v>
+      </c>
+      <c r="C9">
+        <v>42.83</v>
+      </c>
+      <c r="D9">
+        <v>5.32</v>
+      </c>
+      <c r="E9">
+        <v>26.61</v>
+      </c>
+      <c r="F9">
+        <v>7.76</v>
+      </c>
+      <c r="G9">
+        <v>38.82</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>45475.989675925928</v>
+      </c>
+      <c r="B10">
+        <v>10.54</v>
+      </c>
+      <c r="C10">
+        <v>52.71</v>
+      </c>
+      <c r="D10">
+        <v>6.81</v>
+      </c>
+      <c r="E10">
+        <v>34.03</v>
+      </c>
+      <c r="F10">
+        <v>6.94</v>
+      </c>
+      <c r="G10">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>45476.879537037035</v>
+      </c>
+      <c r="B11">
+        <v>7.37</v>
+      </c>
+      <c r="C11">
+        <v>36.86</v>
+      </c>
+      <c r="D11">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="E11">
+        <v>20.3</v>
+      </c>
+      <c r="F11">
+        <v>5.48</v>
+      </c>
+      <c r="G11">
+        <v>27.39</v>
+      </c>
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45477.449652777781</v>
+      </c>
+      <c r="B12">
+        <v>5.27</v>
+      </c>
+      <c r="C12">
+        <v>26.35</v>
+      </c>
+      <c r="D12">
+        <v>4.84</v>
+      </c>
+      <c r="E12">
+        <v>24.19</v>
+      </c>
+      <c r="F12">
+        <v>5.17</v>
+      </c>
+      <c r="G12">
+        <v>25.84</v>
+      </c>
+      <c r="H12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45477.525057870371</v>
+      </c>
+      <c r="B13">
+        <v>6.18</v>
+      </c>
+      <c r="C13">
+        <v>30.88</v>
+      </c>
+      <c r="D13">
+        <v>15.57</v>
+      </c>
+      <c r="E13">
+        <v>20.56</v>
+      </c>
+      <c r="F13">
+        <v>5.13</v>
+      </c>
+      <c r="G13">
+        <v>25.63</v>
+      </c>
+      <c r="H13" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>